<commit_message>
Add COUNTIF examples and images to lecture
Expanded the MCfCL-06-Lecture.md with detailed COUNTIF usage examples and added three illustrative images (fig-09.png, fig-10.png, fig-11.png). Updated Book1.xlsx to support new examples.
</commit_message>
<xml_diff>
--- a/MCfCL-06-Lecture/Book1.xlsx
+++ b/MCfCL-06-Lecture/Book1.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tetsu\github\2025-SIT-MCfCL\MCfCL-06-Lecture\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0E7BF742-8540-44FC-AEC6-86C9B8B3F907}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E55FACB5-6CBE-4F9A-A2C1-6E368069B8C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5970" yWindow="10950" windowWidth="22380" windowHeight="15225" activeTab="3" xr2:uid="{AED3A12A-F503-4655-B8C0-624A7FCB9B9C}"/>
+    <workbookView xWindow="9090" yWindow="11955" windowWidth="22380" windowHeight="15225" activeTab="4" xr2:uid="{AED3A12A-F503-4655-B8C0-624A7FCB9B9C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet2 (2)" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet3" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="34">
   <si>
     <t>合格点</t>
     <rPh sb="0" eb="3">
@@ -119,6 +120,86 @@
   </si>
   <si>
     <t>COUNTBLANK</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>出欠</t>
+    <rPh sb="0" eb="2">
+      <t>シュッケツ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>出席</t>
+    <rPh sb="0" eb="2">
+      <t>シュッセキ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>欠席</t>
+    <rPh sb="0" eb="2">
+      <t>ケッセキ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>出席</t>
+    <rPh sb="0" eb="2">
+      <t>シュ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>欠席</t>
+    <rPh sb="0" eb="2">
+      <t>ケ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>例1</t>
+    <rPh sb="0" eb="1">
+      <t>レイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>例2</t>
+    <rPh sb="0" eb="1">
+      <t>レイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>例3</t>
+    <rPh sb="0" eb="1">
+      <t>レイ</t>
+    </rPh>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -189,7 +270,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -204,6 +285,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -866,8 +950,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABC301B8-D4D9-4A83-9944-CFFCF90D8900}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection sqref="A1:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -989,4 +1073,162 @@
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{370580C8-504B-417D-B1DF-B88A73B9BD6D}">
+  <dimension ref="A1:F10"/>
+  <sheetViews>
+    <sheetView showFormulas="1" tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="5" width="3.875" customWidth="1"/>
+    <col min="6" max="6" width="15.75" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="1">
+        <v>75</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3">
+        <v>3</v>
+      </c>
+      <c r="F3">
+        <f>COUNTIF(B3:B10,"&gt;=60")</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="1">
+        <v>51</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <f>COUNTIF(B3:B10,"&gt;="&amp;$B$1)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+      <c r="F5">
+        <f>COUNTIF(C3:C10,"出席")</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="1">
+        <v>83</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="1">
+        <v>44</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="1">
+        <v>72</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>